<commit_message>
bug fix & don't overwrite file
</commit_message>
<xml_diff>
--- a/files/SBF_120_Aggregated_trend.xlsx
+++ b/files/SBF_120_Aggregated_trend.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Timestamp</t>
   </si>
@@ -92,6 +92,48 @@
   </si>
   <si>
     <t>11 Jan 2024 - 15:51 CET</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 17:52 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:07 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:08 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:09 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:10 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:11 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:12 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:13 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:14 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:15 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:16 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:17 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:18 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:19 UTC</t>
   </si>
 </sst>
 </file>
@@ -449,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -655,6 +697,118 @@
         <v>-68</v>
       </c>
     </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>-46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>-46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>-43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
timestamp added in col name
</commit_message>
<xml_diff>
--- a/files/SBF_120_Aggregated_trend.xlsx
+++ b/files/SBF_120_Aggregated_trend.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Timestamp</t>
   </si>
@@ -134,6 +134,69 @@
   </si>
   <si>
     <t>20 Jan 2024 - 18:19 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:44 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:47 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:48 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:49 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:50 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:51 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:52 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:53 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:54 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:55 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:56 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:57 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:58 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 18:59 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:00 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:01 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:02 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:03 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:04 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:05 UTC</t>
+  </si>
+  <si>
+    <t>20 Jan 2024 - 19:06 UTC</t>
   </si>
 </sst>
 </file>
@@ -491,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -809,6 +872,182 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>